<commit_message>
fixing Mod 4 errors
</commit_message>
<xml_diff>
--- a/module-4/amos_TestPlan.xlsx
+++ b/module-4/amos_TestPlan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jorda\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\csd\csd-380\module-4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35462A0A-0610-49E5-BE86-0CD8B52ED82F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E35B3617-BFA4-4D65-9D38-91F0E31B91FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-135" windowWidth="29040" windowHeight="15990" xr2:uid="{C44015CB-5479-481E-AB1A-ED3A8C124C36}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="61">
   <si>
     <r>
       <t>Project:</t>
@@ -212,32 +212,6 @@
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">&lt;2025/1/30&gt; </t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Peer tester: </t>
-  </si>
-  <si>
-    <r>
-      <t>Date tested:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>&lt;yyyy/mm/dd&gt;</t>
     </r>
   </si>
   <si>
@@ -694,25 +668,25 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -727,13 +701,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1562,7 +1536,7 @@
   <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+      <selection activeCell="D36" sqref="D36:E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="28.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1600,61 +1574,61 @@
       <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="23"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
-      <c r="B6" s="15" t="s">
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="14"/>
+    </row>
+    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="15"/>
+      <c r="B6" s="10" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E6" s="18"/>
     </row>
     <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="14"/>
-      <c r="B7" s="16"/>
+      <c r="A7" s="16"/>
+      <c r="B7" s="11"/>
       <c r="C7" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E7" s="20"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="D8" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="E8" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="15" t="s">
+    </row>
+    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="7" t="s">
         <v>15</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="16"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="7" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="149.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1662,16 +1636,16 @@
         <v>1</v>
       </c>
       <c r="B10" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>20</v>
-      </c>
       <c r="E10" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="67.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1679,16 +1653,16 @@
         <v>2</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1696,16 +1670,16 @@
         <v>3</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="39" thickBot="1" x14ac:dyDescent="0.3">
@@ -1713,88 +1687,88 @@
         <v>4</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="12"/>
+        <v>25</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="23"/>
     </row>
     <row r="15" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="14"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="15"/>
+      <c r="B16" s="10" t="s">
         <v>29</v>
-      </c>
-      <c r="B15" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="23"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
-      <c r="B16" s="15" t="s">
-        <v>31</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>10</v>
+        <v>59</v>
       </c>
       <c r="E16" s="18"/>
     </row>
     <row r="17" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="14"/>
-      <c r="B17" s="16"/>
+      <c r="A17" s="16"/>
+      <c r="B17" s="11"/>
       <c r="C17" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D17" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="E17" s="20"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E17" s="20"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="15" t="s">
+      <c r="C18" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="15" t="s">
+      <c r="D18" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="E18" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="15" t="s">
+    </row>
+    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="11"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="7" t="s">
         <v>15</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="16"/>
-      <c r="B19" s="16"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
-      <c r="E19" s="7" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1802,16 +1776,16 @@
         <v>1</v>
       </c>
       <c r="B20" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>20</v>
-      </c>
       <c r="E20" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="81.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1819,16 +1793,16 @@
         <v>2</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="90.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1836,16 +1810,16 @@
         <v>3</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1853,16 +1827,16 @@
         <v>4</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="99" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1870,86 +1844,86 @@
         <v>5</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B25" s="10"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="12"/>
+        <v>25</v>
+      </c>
+      <c r="B25" s="21"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="23"/>
     </row>
     <row r="26" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="14"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="15"/>
+      <c r="B27" s="10" t="s">
         <v>40</v>
-      </c>
-      <c r="B26" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="C26" s="22"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="23"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="13"/>
-      <c r="B27" s="15" t="s">
-        <v>42</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D27" s="17" t="s">
-        <v>10</v>
+        <v>59</v>
       </c>
       <c r="E27" s="18"/>
     </row>
     <row r="28" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="14"/>
-      <c r="B28" s="16"/>
+      <c r="A28" s="16"/>
+      <c r="B28" s="11"/>
       <c r="C28" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D28" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="E28" s="20"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E28" s="20"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="15" t="s">
+      <c r="C29" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B29" s="15" t="s">
+      <c r="D29" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C29" s="15" t="s">
+      <c r="E29" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D29" s="15" t="s">
+    </row>
+    <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="11"/>
+      <c r="B30" s="11"/>
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="7" t="s">
         <v>15</v>
-      </c>
-      <c r="E29" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="16"/>
-      <c r="B30" s="16"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="7" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -1957,16 +1931,16 @@
         <v>1</v>
       </c>
       <c r="B31" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C31" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D31" s="9" t="s">
-        <v>20</v>
-      </c>
       <c r="E31" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1974,16 +1948,16 @@
         <v>2</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="98.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1991,86 +1965,86 @@
         <v>3</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E33" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B34" s="10"/>
-      <c r="C34" s="11"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="12"/>
+        <v>25</v>
+      </c>
+      <c r="B34" s="21"/>
+      <c r="C34" s="22"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="23"/>
     </row>
     <row r="35" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C35" s="13"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="14"/>
+    </row>
+    <row r="36" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="15"/>
+      <c r="B36" s="10" t="s">
         <v>47</v>
-      </c>
-      <c r="B35" s="21" t="s">
-        <v>48</v>
-      </c>
-      <c r="C35" s="22"/>
-      <c r="D35" s="22"/>
-      <c r="E35" s="23"/>
-    </row>
-    <row r="36" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="13"/>
-      <c r="B36" s="15" t="s">
-        <v>49</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D36" s="17" t="s">
-        <v>10</v>
+        <v>59</v>
       </c>
       <c r="E36" s="18"/>
     </row>
     <row r="37" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="14"/>
-      <c r="B37" s="16"/>
+      <c r="A37" s="16"/>
+      <c r="B37" s="11"/>
       <c r="C37" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D37" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="E37" s="20"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B38" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E37" s="20"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="15" t="s">
+      <c r="C38" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B38" s="15" t="s">
+      <c r="D38" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C38" s="15" t="s">
+      <c r="E38" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D38" s="15" t="s">
+    </row>
+    <row r="39" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="11"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="7" t="s">
         <v>15</v>
-      </c>
-      <c r="E38" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="16"/>
-      <c r="B39" s="16"/>
-      <c r="C39" s="16"/>
-      <c r="D39" s="16"/>
-      <c r="E39" s="7" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="63.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2078,86 +2052,86 @@
         <v>1</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B41" s="10"/>
-      <c r="C41" s="11"/>
-      <c r="D41" s="11"/>
-      <c r="E41" s="12"/>
+        <v>25</v>
+      </c>
+      <c r="B41" s="21"/>
+      <c r="C41" s="22"/>
+      <c r="D41" s="22"/>
+      <c r="E41" s="23"/>
     </row>
     <row r="42" spans="1:5" ht="21" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B42" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="C42" s="13"/>
+      <c r="D42" s="13"/>
+      <c r="E42" s="14"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="15"/>
+      <c r="B43" s="10" t="s">
         <v>52</v>
-      </c>
-      <c r="B42" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="C42" s="22"/>
-      <c r="D42" s="22"/>
-      <c r="E42" s="23"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="13"/>
-      <c r="B43" s="15" t="s">
-        <v>54</v>
       </c>
       <c r="C43" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D43" s="17" t="s">
-        <v>10</v>
+        <v>59</v>
       </c>
       <c r="E43" s="18"/>
     </row>
     <row r="44" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="14"/>
-      <c r="B44" s="16"/>
+      <c r="A44" s="16"/>
+      <c r="B44" s="11"/>
       <c r="C44" s="7" t="s">
         <v>9</v>
       </c>
       <c r="D44" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="E44" s="20"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B45" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E44" s="20"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="15" t="s">
+      <c r="C45" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B45" s="15" t="s">
+      <c r="D45" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C45" s="15" t="s">
+      <c r="E45" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D45" s="15" t="s">
+    </row>
+    <row r="46" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="11"/>
+      <c r="B46" s="11"/>
+      <c r="C46" s="11"/>
+      <c r="D46" s="11"/>
+      <c r="E46" s="7" t="s">
         <v>15</v>
-      </c>
-      <c r="E45" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="16"/>
-      <c r="B46" s="16"/>
-      <c r="C46" s="16"/>
-      <c r="D46" s="16"/>
-      <c r="E46" s="7" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="47" spans="1:5" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -2165,16 +2139,16 @@
         <v>1</v>
       </c>
       <c r="B47" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D47" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C47" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D47" s="9" t="s">
-        <v>20</v>
-      </c>
       <c r="E47" s="9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="48" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2182,16 +2156,16 @@
         <v>2</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C48" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E48" s="9" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2199,38 +2173,58 @@
         <v>3</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C49" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D49" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E49" s="9" t="s">
         <v>58</v>
-      </c>
-      <c r="D49" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E49" s="9" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B50" s="10"/>
-      <c r="C50" s="11"/>
-      <c r="D50" s="11"/>
-      <c r="E50" s="12"/>
+        <v>25</v>
+      </c>
+      <c r="B50" s="21"/>
+      <c r="C50" s="22"/>
+      <c r="D50" s="22"/>
+      <c r="E50" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="B5:E5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="B50:E50"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="B42:E42"/>
+    <mergeCell ref="B34:E34"/>
+    <mergeCell ref="B35:E35"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="B41:E41"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
     <mergeCell ref="B26:E26"/>
     <mergeCell ref="B14:E14"/>
     <mergeCell ref="B15:E15"/>
@@ -2243,35 +2237,15 @@
     <mergeCell ref="C18:C19"/>
     <mergeCell ref="D18:D19"/>
     <mergeCell ref="B25:E25"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="B42:E42"/>
-    <mergeCell ref="B34:E34"/>
-    <mergeCell ref="B35:E35"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="B41:E41"/>
-    <mergeCell ref="B50:E50"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="B5:E5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D7:E7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>